<commit_message>
edited sample summer sem xlsx file
</commit_message>
<xml_diff>
--- a/sample_summer_sems.xlsx
+++ b/sample_summer_sems.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t xml:space="preserve">COURSE OWNER</t>
   </si>
@@ -83,6 +83,57 @@
   </si>
   <si>
     <t xml:space="preserve">COURSE STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">someone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some tut hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some pracs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some projs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some credits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some erpid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some emp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some</t>
   </si>
 </sst>
 </file>
@@ -207,25 +258,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="7" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.8056680161943"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.5627530364372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.004048582996"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,27 +347,72 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>

</xml_diff>